<commit_message>
Funcion de cargar Proveedores lista
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdeaPad S340 1TB SSD\Desktop\Migracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8A62D2-A81B-4046-BAE9-D9CDDCEEC9E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799F683D-697A-4190-AE36-85017AA3A605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54402053-65C1-4D99-A2CE-BF6AA8FE1990}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$128</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="142">
   <si>
     <t>Productos</t>
   </si>
@@ -472,12 +475,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -492,10 +501,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,13 +822,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA78103-BE44-47D8-9C2A-DE8C26E06AED}">
   <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F91" workbookViewId="0">
-      <selection activeCell="H126" sqref="H126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -844,22 +854,22 @@
       <c r="E1" t="s">
         <v>136</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>137</v>
       </c>
       <c r="G1" t="s">
         <v>138</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -868,7 +878,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -879,10 +892,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -892,6 +905,9 @@
       </c>
       <c r="E3" t="s">
         <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -905,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -914,21 +930,21 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -937,13 +953,13 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
-      </c>
-      <c r="H5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -951,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -960,21 +976,21 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
-      </c>
-      <c r="H6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -983,21 +999,21 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G7" t="s">
         <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1006,21 +1022,21 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G8" t="s">
         <v>3</v>
-      </c>
-      <c r="H8" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -1029,21 +1045,21 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1054,19 +1070,19 @@
       <c r="E10" t="s">
         <v>3</v>
       </c>
+      <c r="F10" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="G10" t="s">
         <v>3</v>
-      </c>
-      <c r="H10" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1086,10 +1102,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1109,10 +1125,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1135,7 +1151,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1150,15 +1166,15 @@
         <v>140</v>
       </c>
       <c r="G14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1178,10 +1194,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1190,21 +1206,21 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G16" t="s">
         <v>3</v>
       </c>
-      <c r="H16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1222,12 +1238,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1242,15 +1258,15 @@
         <v>140</v>
       </c>
       <c r="G18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1268,12 +1284,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1288,15 +1304,15 @@
         <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1305,21 +1321,21 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="G21" t="s">
         <v>3</v>
       </c>
-      <c r="H21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -1334,15 +1350,15 @@
         <v>140</v>
       </c>
       <c r="G22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1357,15 +1373,15 @@
         <v>140</v>
       </c>
       <c r="G23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -1383,15 +1399,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
         <v>2</v>
@@ -1406,15 +1422,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
         <v>2</v>
@@ -1426,15 +1442,15 @@
         <v>140</v>
       </c>
       <c r="G26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -1452,12 +1468,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -1472,18 +1488,18 @@
         <v>140</v>
       </c>
       <c r="G28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
         <v>2</v>
@@ -1498,12 +1514,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -1521,12 +1537,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -1544,12 +1560,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -1572,7 +1588,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -1595,10 +1611,10 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
         <v>2</v>
@@ -1618,10 +1634,10 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>2</v>
@@ -1633,15 +1649,15 @@
         <v>140</v>
       </c>
       <c r="G35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -1664,10 +1680,10 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
         <v>2</v>
@@ -1679,7 +1695,7 @@
         <v>140</v>
       </c>
       <c r="G37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1687,10 +1703,10 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
         <v>2</v>
@@ -1702,7 +1718,7 @@
         <v>140</v>
       </c>
       <c r="G38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1710,10 +1726,10 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
@@ -1733,7 +1749,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -1756,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -1771,15 +1787,15 @@
         <v>140</v>
       </c>
       <c r="G41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -1794,15 +1810,15 @@
         <v>140</v>
       </c>
       <c r="G42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -1822,10 +1838,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -1845,10 +1861,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -1868,13 +1884,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46" t="s">
         <v>2</v>
@@ -1886,15 +1902,15 @@
         <v>140</v>
       </c>
       <c r="G46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -1914,13 +1930,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
@@ -1937,13 +1953,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49" t="s">
         <v>2</v>
@@ -1955,18 +1971,18 @@
         <v>140</v>
       </c>
       <c r="G49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
         <v>2</v>
@@ -1978,18 +1994,18 @@
         <v>140</v>
       </c>
       <c r="G50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
@@ -2001,18 +2017,18 @@
         <v>140</v>
       </c>
       <c r="G51" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" t="s">
         <v>2</v>
@@ -2024,7 +2040,7 @@
         <v>140</v>
       </c>
       <c r="G52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2032,10 +2048,10 @@
         <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D53" t="s">
         <v>2</v>
@@ -2052,13 +2068,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
@@ -2070,7 +2086,7 @@
         <v>140</v>
       </c>
       <c r="G54" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2078,10 +2094,10 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -2093,7 +2109,7 @@
         <v>140</v>
       </c>
       <c r="G55" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2101,7 +2117,7 @@
         <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
@@ -2111,9 +2127,6 @@
       </c>
       <c r="E56" t="s">
         <v>3</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G56" t="s">
         <v>3</v>
@@ -2124,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
@@ -2139,7 +2152,7 @@
         <v>140</v>
       </c>
       <c r="G57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2147,10 +2160,10 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" t="s">
         <v>2</v>
@@ -2162,18 +2175,18 @@
         <v>140</v>
       </c>
       <c r="G58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
         <v>2</v>
@@ -2185,7 +2198,7 @@
         <v>140</v>
       </c>
       <c r="G59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2193,10 +2206,10 @@
         <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
         <v>2</v>
@@ -2208,18 +2221,18 @@
         <v>140</v>
       </c>
       <c r="G60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
@@ -2239,7 +2252,7 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C62" t="s">
         <v>3</v>
@@ -2254,15 +2267,15 @@
         <v>140</v>
       </c>
       <c r="G62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
@@ -2285,10 +2298,10 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
         <v>2</v>
@@ -2300,7 +2313,7 @@
         <v>140</v>
       </c>
       <c r="G64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2308,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C65" t="s">
         <v>2</v>
@@ -2319,8 +2332,11 @@
       <c r="E65" t="s">
         <v>3</v>
       </c>
+      <c r="F65" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="G65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2328,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
@@ -2351,10 +2367,10 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
         <v>2</v>
@@ -2366,7 +2382,7 @@
         <v>140</v>
       </c>
       <c r="G67" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2374,10 +2390,10 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C68" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D68" t="s">
         <v>2</v>
@@ -2385,11 +2401,8 @@
       <c r="E68" t="s">
         <v>3</v>
       </c>
-      <c r="F68" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="G68" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2397,10 +2410,10 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C69" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" t="s">
         <v>2</v>
@@ -2408,19 +2421,22 @@
       <c r="E69" t="s">
         <v>3</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" t="s">
         <v>140</v>
       </c>
       <c r="G69" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="H69" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C70" t="s">
         <v>2</v>
@@ -2431,7 +2447,7 @@
       <c r="E70" t="s">
         <v>3</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" t="s">
         <v>140</v>
       </c>
       <c r="G70" t="s">
@@ -2443,10 +2459,10 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
         <v>2</v>
@@ -2454,7 +2470,7 @@
       <c r="E71" t="s">
         <v>3</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" t="s">
         <v>140</v>
       </c>
       <c r="G71" t="s">
@@ -2463,13 +2479,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
         <v>2</v>
@@ -2477,11 +2493,11 @@
       <c r="E72" t="s">
         <v>3</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" t="s">
         <v>140</v>
       </c>
       <c r="G72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2489,7 +2505,7 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C73" t="s">
         <v>2</v>
@@ -2500,7 +2516,7 @@
       <c r="E73" t="s">
         <v>3</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F73" t="s">
         <v>140</v>
       </c>
       <c r="G73" t="s">
@@ -2512,10 +2528,10 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C74" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D74" t="s">
         <v>2</v>
@@ -2523,11 +2539,11 @@
       <c r="E74" t="s">
         <v>3</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" t="s">
         <v>140</v>
       </c>
       <c r="G74" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2535,7 +2551,7 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C75" t="s">
         <v>2</v>
@@ -2546,7 +2562,7 @@
       <c r="E75" t="s">
         <v>3</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F75" t="s">
         <v>140</v>
       </c>
       <c r="G75" t="s">
@@ -2558,10 +2574,10 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
         <v>2</v>
@@ -2569,11 +2585,11 @@
       <c r="E76" t="s">
         <v>3</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" t="s">
         <v>140</v>
       </c>
       <c r="G76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2581,10 +2597,10 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
         <v>2</v>
@@ -2592,8 +2608,11 @@
       <c r="E77" t="s">
         <v>3</v>
       </c>
+      <c r="F77" t="s">
+        <v>140</v>
+      </c>
       <c r="G77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -2601,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C78" t="s">
         <v>3</v>
@@ -2617,20 +2636,17 @@
       </c>
       <c r="G78" t="s">
         <v>3</v>
-      </c>
-      <c r="H78" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C79" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D79" t="s">
         <v>2</v>
@@ -2642,7 +2658,7 @@
         <v>140</v>
       </c>
       <c r="G79" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -2650,10 +2666,10 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C80" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D80" t="s">
         <v>2</v>
@@ -2665,7 +2681,7 @@
         <v>140</v>
       </c>
       <c r="G80" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2673,10 +2689,10 @@
         <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C81" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" t="s">
         <v>2</v>
@@ -2688,7 +2704,7 @@
         <v>140</v>
       </c>
       <c r="G81" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2696,10 +2712,10 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D82" t="s">
         <v>2</v>
@@ -2711,7 +2727,7 @@
         <v>140</v>
       </c>
       <c r="G82" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2719,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
         <v>3</v>
@@ -2742,10 +2758,10 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C84" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D84" t="s">
         <v>2</v>
@@ -2757,7 +2773,7 @@
         <v>140</v>
       </c>
       <c r="G84" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2765,10 +2781,10 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D85" t="s">
         <v>2</v>
@@ -2776,11 +2792,8 @@
       <c r="E85" t="s">
         <v>3</v>
       </c>
-      <c r="F85" t="s">
-        <v>140</v>
-      </c>
       <c r="G85" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2788,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C86" t="s">
         <v>2</v>
@@ -2803,15 +2816,15 @@
         <v>140</v>
       </c>
       <c r="G86" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
         <v>3</v>
@@ -2834,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C88" t="s">
         <v>3</v>
@@ -2849,7 +2862,7 @@
         <v>140</v>
       </c>
       <c r="G88" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2857,7 +2870,7 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C89" t="s">
         <v>3</v>
@@ -2872,7 +2885,7 @@
         <v>140</v>
       </c>
       <c r="G89" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2880,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="B90" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C90" t="s">
         <v>3</v>
@@ -2895,15 +2908,15 @@
         <v>140</v>
       </c>
       <c r="G90" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C91" t="s">
         <v>3</v>
@@ -2918,18 +2931,18 @@
         <v>140</v>
       </c>
       <c r="G91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C92" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D92" t="s">
         <v>2</v>
@@ -2949,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
         <v>3</v>
@@ -2964,7 +2977,7 @@
         <v>140</v>
       </c>
       <c r="G93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -2972,7 +2985,7 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C94" t="s">
         <v>3</v>
@@ -2982,6 +2995,9 @@
       </c>
       <c r="E94" t="s">
         <v>3</v>
+      </c>
+      <c r="F94" t="s">
+        <v>140</v>
       </c>
       <c r="G94" t="s">
         <v>3</v>
@@ -2992,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C95" t="s">
         <v>2</v>
@@ -3007,7 +3023,7 @@
         <v>140</v>
       </c>
       <c r="G95" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3015,7 +3031,7 @@
         <v>4</v>
       </c>
       <c r="B96" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C96" t="s">
         <v>3</v>
@@ -3033,15 +3049,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>0</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
         <v>2</v>
@@ -3049,22 +3065,19 @@
       <c r="E97" t="s">
         <v>3</v>
       </c>
-      <c r="F97" t="s">
-        <v>140</v>
-      </c>
       <c r="G97" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C98" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D98" t="s">
         <v>2</v>
@@ -3076,41 +3089,41 @@
         <v>140</v>
       </c>
       <c r="G98" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>0</v>
       </c>
       <c r="B99" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C99" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
       </c>
       <c r="E99" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F99" t="s">
+        <v>140</v>
       </c>
       <c r="G99" t="s">
         <v>3</v>
       </c>
-      <c r="H99" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>0</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C100" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D100" t="s">
         <v>2</v>
@@ -3125,15 +3138,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>4</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C101" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
@@ -3148,12 +3161,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>4</v>
       </c>
       <c r="B102" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C102" t="s">
         <v>2</v>
@@ -3168,18 +3181,18 @@
         <v>140</v>
       </c>
       <c r="G102" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>0</v>
       </c>
       <c r="B103" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C103" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D103" t="s">
         <v>2</v>
@@ -3187,19 +3200,16 @@
       <c r="E103" t="s">
         <v>3</v>
       </c>
-      <c r="F103" t="s">
-        <v>140</v>
-      </c>
       <c r="G103" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>0</v>
       </c>
       <c r="B104" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C104" t="s">
         <v>3</v>
@@ -3210,22 +3220,19 @@
       <c r="E104" t="s">
         <v>3</v>
       </c>
-      <c r="F104" t="s">
-        <v>140</v>
-      </c>
       <c r="G104" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>0</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C105" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D105" t="s">
         <v>2</v>
@@ -3237,18 +3244,18 @@
         <v>140</v>
       </c>
       <c r="G105" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B106" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C106" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D106" t="s">
         <v>2</v>
@@ -3263,15 +3270,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C107" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -3283,12 +3290,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C108" t="s">
         <v>2</v>
@@ -3299,22 +3306,19 @@
       <c r="E108" t="s">
         <v>3</v>
       </c>
-      <c r="F108" t="s">
-        <v>140</v>
-      </c>
       <c r="G108" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>0</v>
       </c>
       <c r="B109" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C109" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D109" t="s">
         <v>2</v>
@@ -3329,12 +3333,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C110" t="s">
         <v>2</v>
@@ -3343,21 +3347,21 @@
         <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F110" t="s">
+        <v>140</v>
       </c>
       <c r="G110" t="s">
         <v>3</v>
       </c>
-      <c r="H110" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>0</v>
       </c>
       <c r="B111" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C111" t="s">
         <v>2</v>
@@ -3366,21 +3370,21 @@
         <v>2</v>
       </c>
       <c r="E111" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F111" t="s">
+        <v>140</v>
       </c>
       <c r="G111" t="s">
         <v>3</v>
       </c>
-      <c r="H111" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C112" t="s">
         <v>2</v>
@@ -3395,15 +3399,15 @@
         <v>140</v>
       </c>
       <c r="G112" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B113" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C113" t="s">
         <v>2</v>
@@ -3414,19 +3418,16 @@
       <c r="E113" t="s">
         <v>3</v>
       </c>
-      <c r="F113" t="s">
-        <v>140</v>
-      </c>
       <c r="G113" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B114" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="C114" t="s">
         <v>2</v>
@@ -3437,11 +3438,11 @@
       <c r="E114" t="s">
         <v>3</v>
       </c>
-      <c r="F114" t="s">
-        <v>140</v>
-      </c>
       <c r="G114" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="H114" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -3449,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="B115" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C115" t="s">
         <v>2</v>
@@ -3469,10 +3470,10 @@
         <v>0</v>
       </c>
       <c r="B116" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="C116" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D116" t="s">
         <v>2</v>
@@ -3489,22 +3490,22 @@
         <v>0</v>
       </c>
       <c r="B117" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D117" t="s">
         <v>2</v>
       </c>
       <c r="E117" t="s">
-        <v>3</v>
-      </c>
-      <c r="F117" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="G117" t="s">
         <v>3</v>
+      </c>
+      <c r="H117" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3512,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="B118" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="C118" t="s">
         <v>2</v>
@@ -3521,33 +3522,36 @@
         <v>2</v>
       </c>
       <c r="E118" t="s">
-        <v>3</v>
-      </c>
-      <c r="F118" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="G118" t="s">
         <v>3</v>
+      </c>
+      <c r="H118" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B119" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="C119" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D119" t="s">
         <v>2</v>
       </c>
       <c r="E119" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G119" t="s">
         <v>3</v>
+      </c>
+      <c r="H119" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -3555,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="B120" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
       <c r="C120" t="s">
         <v>2</v>
@@ -3564,10 +3568,13 @@
         <v>2</v>
       </c>
       <c r="E120" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G120" t="s">
         <v>3</v>
+      </c>
+      <c r="H120" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3575,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="B121" t="s">
-        <v>124</v>
+        <v>9</v>
       </c>
       <c r="C121" t="s">
         <v>2</v>
@@ -3584,21 +3591,21 @@
         <v>2</v>
       </c>
       <c r="E121" t="s">
-        <v>3</v>
-      </c>
-      <c r="F121" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="G121" t="s">
         <v>3</v>
+      </c>
+      <c r="H121" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B122" t="s">
-        <v>125</v>
+        <v>10</v>
       </c>
       <c r="C122" t="s">
         <v>2</v>
@@ -3607,13 +3614,13 @@
         <v>2</v>
       </c>
       <c r="E122" t="s">
-        <v>3</v>
-      </c>
-      <c r="F122" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="G122" t="s">
         <v>3</v>
+      </c>
+      <c r="H122" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -3621,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="B123" t="s">
-        <v>126</v>
+        <v>11</v>
       </c>
       <c r="C123" t="s">
         <v>2</v>
@@ -3630,21 +3637,21 @@
         <v>2</v>
       </c>
       <c r="E123" t="s">
-        <v>3</v>
-      </c>
-      <c r="F123" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="G123" t="s">
         <v>3</v>
+      </c>
+      <c r="H123" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B124" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="C124" t="s">
         <v>2</v>
@@ -3653,13 +3660,13 @@
         <v>2</v>
       </c>
       <c r="E124" t="s">
-        <v>3</v>
-      </c>
-      <c r="F124" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="G124" t="s">
         <v>3</v>
+      </c>
+      <c r="H124" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -3667,7 +3674,7 @@
         <v>0</v>
       </c>
       <c r="B125" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="C125" t="s">
         <v>2</v>
@@ -3676,10 +3683,13 @@
         <v>2</v>
       </c>
       <c r="E125" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G125" t="s">
         <v>3</v>
+      </c>
+      <c r="H125" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -3687,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="B126" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="C126" t="s">
         <v>2</v>
@@ -3696,7 +3706,7 @@
         <v>2</v>
       </c>
       <c r="E126" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G126" t="s">
         <v>3</v>
@@ -3710,7 +3720,7 @@
         <v>0</v>
       </c>
       <c r="B127" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C127" t="s">
         <v>2</v>
@@ -3719,10 +3729,13 @@
         <v>2</v>
       </c>
       <c r="E127" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G127" t="s">
         <v>3</v>
+      </c>
+      <c r="H127" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -3730,7 +3743,7 @@
         <v>0</v>
       </c>
       <c r="B128" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C128" t="s">
         <v>2</v>
@@ -3739,13 +3752,21 @@
         <v>2</v>
       </c>
       <c r="E128" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G128" t="s">
         <v>3</v>
       </c>
+      <c r="H128" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H128" xr:uid="{E25E4F31-0451-410C-A797-26A43EA3FAB4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H128">
+      <sortCondition descending="1" ref="E2:E128"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>